<commit_message>
fix: removed files unnecessary
</commit_message>
<xml_diff>
--- a/resultados/nfs/teste_7gb.xlsx
+++ b/resultados/nfs/teste_7gb.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="teste_7gb" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="teste_7gb_2" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -312,10 +312,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="17.88"/>
-    <col customWidth="1" min="7" max="7" width="19.0"/>
-    <col customWidth="1" min="8" max="8" width="16.25"/>
-    <col customWidth="1" min="9" max="9" width="20.63"/>
+    <col customWidth="1" min="6" max="6" width="16.75"/>
+    <col customWidth="1" min="7" max="7" width="17.63"/>
+    <col customWidth="1" min="8" max="8" width="18.13"/>
+    <col customWidth="1" min="9" max="9" width="22.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -346,718 +346,718 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>34.31</v>
+        <v>48.32</v>
       </c>
       <c r="B2" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C2" s="1">
-        <v>11.23</v>
+        <v>11.56</v>
       </c>
       <c r="D2" s="3">
-        <v>0.32</v>
+        <v>0.23</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" ref="F2:I2" si="1">AVERAGE(A2:A51)</f>
-        <v>35.6916</v>
+        <v>23.963</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" si="1"/>
-        <v>0.0302</v>
+        <v>0.0262</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" si="1"/>
-        <v>11.662</v>
+        <v>10.8528</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" si="1"/>
-        <v>0.3228</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>34.15</v>
+        <v>28.37</v>
       </c>
       <c r="B3" s="1">
         <v>0.02</v>
       </c>
       <c r="C3" s="1">
-        <v>11.55</v>
+        <v>10.83</v>
       </c>
       <c r="D3" s="3">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>35.15</v>
+        <v>31.64</v>
       </c>
       <c r="B4" s="1">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="C4" s="1">
-        <v>12.15</v>
+        <v>11.66</v>
       </c>
       <c r="D4" s="3">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>35.26</v>
+        <v>28.19</v>
       </c>
       <c r="B5" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C5" s="1">
-        <v>11.77</v>
+        <v>11.11</v>
       </c>
       <c r="D5" s="3">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>35.7</v>
+        <v>25.99</v>
       </c>
       <c r="B6" s="1">
         <v>0.03</v>
       </c>
       <c r="C6" s="1">
-        <v>11.21</v>
+        <v>10.75</v>
       </c>
       <c r="D6" s="3">
-        <v>0.31</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>36.96</v>
+        <v>27.54</v>
       </c>
       <c r="B7" s="1">
         <v>0.03</v>
       </c>
       <c r="C7" s="1">
-        <v>11.94</v>
+        <v>10.85</v>
       </c>
       <c r="D7" s="3">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>34.93</v>
+        <v>27.59</v>
       </c>
       <c r="B8" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C8" s="1">
-        <v>11.49</v>
+        <v>12.6</v>
       </c>
       <c r="D8" s="3">
-        <v>0.33</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>35.6</v>
+        <v>26.3</v>
       </c>
       <c r="B9" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C9" s="1">
-        <v>11.75</v>
+        <v>10.86</v>
       </c>
       <c r="D9" s="3">
-        <v>0.33</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>36.71</v>
+        <v>26.3</v>
       </c>
       <c r="B10" s="1">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="C10" s="1">
-        <v>11.19</v>
+        <v>11.49</v>
       </c>
       <c r="D10" s="3">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>33.57</v>
+        <v>25.84</v>
       </c>
       <c r="B11" s="1">
         <v>0.03</v>
       </c>
       <c r="C11" s="1">
-        <v>11.11</v>
+        <v>11.8</v>
       </c>
       <c r="D11" s="3">
-        <v>0.33</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>35.98</v>
+        <v>25.75</v>
       </c>
       <c r="B12" s="1">
         <v>0.03</v>
       </c>
       <c r="C12" s="1">
-        <v>11.25</v>
+        <v>11.08</v>
       </c>
       <c r="D12" s="3">
-        <v>0.31</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>34.27</v>
+        <v>25.79</v>
       </c>
       <c r="B13" s="1">
         <v>0.03</v>
       </c>
       <c r="C13" s="1">
-        <v>11.36</v>
+        <v>11.86</v>
       </c>
       <c r="D13" s="3">
-        <v>0.33</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>37.02</v>
+        <v>25.2</v>
       </c>
       <c r="B14" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C14" s="1">
-        <v>11.45</v>
+        <v>11.08</v>
       </c>
       <c r="D14" s="3">
-        <v>0.31</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>37.39</v>
+        <v>23.96</v>
       </c>
       <c r="B15" s="1">
         <v>0.02</v>
       </c>
       <c r="C15" s="1">
-        <v>11.56</v>
+        <v>10.45</v>
       </c>
       <c r="D15" s="3">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>35.24</v>
+        <v>24.86</v>
       </c>
       <c r="B16" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C16" s="1">
-        <v>11.77</v>
+        <v>10.84</v>
       </c>
       <c r="D16" s="3">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>35.37</v>
+        <v>23.96</v>
       </c>
       <c r="B17" s="1">
         <v>0.03</v>
       </c>
       <c r="C17" s="1">
-        <v>11.34</v>
+        <v>11.11</v>
       </c>
       <c r="D17" s="3">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>33.75</v>
+        <v>24.76</v>
       </c>
       <c r="B18" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C18" s="1">
-        <v>10.97</v>
+        <v>11.97</v>
       </c>
       <c r="D18" s="3">
-        <v>0.32</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>34.05</v>
+        <v>24.16</v>
       </c>
       <c r="B19" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C19" s="1">
-        <v>11.84</v>
+        <v>11.13</v>
       </c>
       <c r="D19" s="3">
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>35.47</v>
+        <v>24.26</v>
       </c>
       <c r="B20" s="1">
         <v>0.03</v>
       </c>
       <c r="C20" s="1">
-        <v>12.64</v>
+        <v>11.58</v>
       </c>
       <c r="D20" s="3">
-        <v>0.35</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>36.7</v>
+        <v>23.49</v>
       </c>
       <c r="B21" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C21" s="1">
-        <v>11.44</v>
+        <v>10.61</v>
       </c>
       <c r="D21" s="3">
-        <v>0.31</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>35.79</v>
+        <v>23.56</v>
       </c>
       <c r="B22" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C22" s="1">
-        <v>11.46</v>
+        <v>10.46</v>
       </c>
       <c r="D22" s="3">
-        <v>0.32</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>37.79</v>
+        <v>23.3</v>
       </c>
       <c r="B23" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C23" s="1">
-        <v>11.36</v>
+        <v>10.93</v>
       </c>
       <c r="D23" s="3">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>36.74</v>
+        <v>23.94</v>
       </c>
       <c r="B24" s="1">
         <v>0.03</v>
       </c>
       <c r="C24" s="1">
-        <v>12.35</v>
+        <v>11.54</v>
       </c>
       <c r="D24" s="3">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>37.7</v>
+        <v>23.14</v>
       </c>
       <c r="B25" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C25" s="1">
-        <v>11.92</v>
+        <v>10.68</v>
       </c>
       <c r="D25" s="3">
-        <v>0.31</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>33.71</v>
+        <v>23.05</v>
       </c>
       <c r="B26" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C26" s="1">
-        <v>11.69</v>
+        <v>10.46</v>
       </c>
       <c r="D26" s="3">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>35.07</v>
+        <v>22.24</v>
       </c>
       <c r="B27" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C27" s="1">
-        <v>11.56</v>
+        <v>10.49</v>
       </c>
       <c r="D27" s="3">
-        <v>0.33</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>37.13</v>
+        <v>22.36</v>
       </c>
       <c r="B28" s="1">
         <v>0.03</v>
       </c>
       <c r="C28" s="1">
-        <v>13.0</v>
+        <v>10.35</v>
       </c>
       <c r="D28" s="3">
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>37.3</v>
+        <v>22.51</v>
       </c>
       <c r="B29" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C29" s="1">
-        <v>13.26</v>
+        <v>10.22</v>
       </c>
       <c r="D29" s="3">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>35.6</v>
+        <v>22.25</v>
       </c>
       <c r="B30" s="1">
         <v>0.03</v>
       </c>
       <c r="C30" s="1">
-        <v>11.78</v>
+        <v>10.74</v>
       </c>
       <c r="D30" s="3">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>36.08</v>
+        <v>22.73</v>
       </c>
       <c r="B31" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C31" s="1">
-        <v>11.66</v>
+        <v>11.16</v>
       </c>
       <c r="D31" s="3">
-        <v>0.32</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>35.7</v>
+        <v>22.09</v>
       </c>
       <c r="B32" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C32" s="1">
-        <v>11.32</v>
+        <v>10.73</v>
       </c>
       <c r="D32" s="3">
-        <v>0.31</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>36.4</v>
+        <v>21.35</v>
       </c>
       <c r="B33" s="1">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="C33" s="1">
-        <v>11.71</v>
+        <v>10.33</v>
       </c>
       <c r="D33" s="3">
-        <v>0.32</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>35.89</v>
+        <v>21.38</v>
       </c>
       <c r="B34" s="1">
         <v>0.02</v>
       </c>
       <c r="C34" s="1">
-        <v>11.6</v>
+        <v>10.21</v>
       </c>
       <c r="D34" s="3">
-        <v>0.32</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>37.82</v>
+        <v>21.26</v>
       </c>
       <c r="B35" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C35" s="1">
-        <v>11.63</v>
+        <v>10.27</v>
       </c>
       <c r="D35" s="3">
-        <v>0.3</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>36.06</v>
+        <v>21.28</v>
       </c>
       <c r="B36" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C36" s="1">
-        <v>11.61</v>
+        <v>10.02</v>
       </c>
       <c r="D36" s="3">
-        <v>0.32</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>35.84</v>
+        <v>21.41</v>
       </c>
       <c r="B37" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C37" s="1">
-        <v>11.62</v>
+        <v>10.4</v>
       </c>
       <c r="D37" s="3">
-        <v>0.32</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>35.63</v>
+        <v>21.75</v>
       </c>
       <c r="B38" s="1">
         <v>0.03</v>
       </c>
       <c r="C38" s="1">
-        <v>11.69</v>
+        <v>10.64</v>
       </c>
       <c r="D38" s="3">
-        <v>0.32</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>36.55</v>
+        <v>22.44</v>
       </c>
       <c r="B39" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C39" s="1">
-        <v>11.83</v>
+        <v>11.4</v>
       </c>
       <c r="D39" s="3">
-        <v>0.32</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>37.67</v>
+        <v>21.72</v>
       </c>
       <c r="B40" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C40" s="1">
-        <v>11.88</v>
+        <v>10.41</v>
       </c>
       <c r="D40" s="3">
-        <v>0.31</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>36.45</v>
+        <v>20.92</v>
       </c>
       <c r="B41" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C41" s="1">
-        <v>12.1</v>
+        <v>10.04</v>
       </c>
       <c r="D41" s="3">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>33.78</v>
+        <v>21.31</v>
       </c>
       <c r="B42" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C42" s="1">
-        <v>11.36</v>
+        <v>10.27</v>
       </c>
       <c r="D42" s="3">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>36.47</v>
+        <v>20.97</v>
       </c>
       <c r="B43" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C43" s="1">
-        <v>11.56</v>
+        <v>10.12</v>
       </c>
       <c r="D43" s="3">
-        <v>0.31</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>33.8</v>
+        <v>20.75</v>
       </c>
       <c r="B44" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C44" s="1">
-        <v>11.38</v>
+        <v>10.02</v>
       </c>
       <c r="D44" s="3">
-        <v>0.33</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>35.92</v>
+        <v>20.97</v>
       </c>
       <c r="B45" s="1">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="C45" s="1">
-        <v>11.75</v>
+        <v>10.3</v>
       </c>
       <c r="D45" s="3">
-        <v>0.32</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1">
-        <v>34.52</v>
+        <v>21.42</v>
       </c>
       <c r="B46" s="1">
         <v>0.03</v>
       </c>
       <c r="C46" s="1">
-        <v>11.25</v>
+        <v>10.96</v>
       </c>
       <c r="D46" s="3">
-        <v>0.32</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1">
-        <v>36.45</v>
+        <v>21.85</v>
       </c>
       <c r="B47" s="1">
         <v>0.03</v>
       </c>
       <c r="C47" s="1">
-        <v>11.59</v>
+        <v>11.5</v>
       </c>
       <c r="D47" s="3">
-        <v>0.31</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1">
-        <v>37.67</v>
+        <v>20.95</v>
       </c>
       <c r="B48" s="1">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="C48" s="1">
-        <v>11.87</v>
+        <v>10.84</v>
       </c>
       <c r="D48" s="3">
-        <v>0.31</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1">
-        <v>33.99</v>
+        <v>21.29</v>
       </c>
       <c r="B49" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C49" s="1">
-        <v>11.42</v>
+        <v>11.05</v>
       </c>
       <c r="D49" s="3">
-        <v>0.33</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1">
-        <v>33.03</v>
+        <v>20.96</v>
       </c>
       <c r="B50" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C50" s="1">
-        <v>11.59</v>
+        <v>10.65</v>
       </c>
       <c r="D50" s="3">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1">
-        <v>34.45</v>
+        <v>20.73</v>
       </c>
       <c r="B51" s="1">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="C51" s="1">
-        <v>11.29</v>
+        <v>10.23</v>
       </c>
       <c r="D51" s="3">
-        <v>0.32</v>
+        <v>0.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>